<commit_message>
extract more papers at level P2, P3
</commit_message>
<xml_diff>
--- a/State of Art_Text Detection & Recognition.xlsx
+++ b/State of Art_Text Detection & Recognition.xlsx
@@ -4,26 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="8475" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="8475" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Papers" sheetId="1" r:id="rId1"/>
     <sheet name="Priority" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Extract P1" sheetId="3" r:id="rId3"/>
+    <sheet name="Extract P2&amp;P3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Extract P1'!$A$6:$G$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Papers!$A$4:$H$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Priority!$A$9:$D$80</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$5:$F$5</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="2">Sheet3!$J$2:$J$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="2">Sheet3!$A$52:$G$52</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="2">'Extract P1'!$J$2:$J$3</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="3">'Extract P2&amp;P3'!$J$1:$J$2</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="2">'Extract P1'!#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="3">'Extract P2&amp;P3'!$A$38:$G$38</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="506">
   <si>
     <t>Title</t>
   </si>
@@ -2551,9 +2555,6 @@
     <t>Signal Processing and Communications Applications</t>
   </si>
   <si>
-    <t>VISUAL</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
@@ -2576,6 +2577,12 @@
   </si>
   <si>
     <t>P4</t>
+  </si>
+  <si>
+    <t>Recent Advances in Visual Information Systems</t>
+  </si>
+  <si>
+    <t>Extract Papers at level P2</t>
   </si>
 </sst>
 </file>
@@ -2711,7 +2718,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3030,7 +3047,7 @@
   <dimension ref="A1:H159"/>
   <sheetViews>
     <sheetView topLeftCell="F133" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B159"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,7 +3099,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E5)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E5)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -3100,7 +3117,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E6)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E6)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -3119,7 +3136,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E7)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E7)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -3138,7 +3155,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E8)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E8)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -3157,7 +3174,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E9)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E9)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -3176,7 +3193,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E10)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E10)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -3195,7 +3212,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E11)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E11)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -3213,9 +3230,9 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="str">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E12)&gt;0),Priority!$B$83)</f>
-        <v>P1</v>
+      <c r="B12" s="1" t="e">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E12)&gt;0),Priority!$B$85)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>97</v>
@@ -3233,7 +3250,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E13)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E13)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -3251,7 +3268,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E14)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E14)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -3269,7 +3286,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E15)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E15)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -3287,7 +3304,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E16)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E16)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -3305,7 +3322,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E17)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E17)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -3323,7 +3340,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E18)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E18)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -3340,9 +3357,9 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E19)&gt;0),Priority!$B$83)</f>
-        <v>#VALUE!</v>
+      <c r="B19" s="1" t="str">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E19)&gt;0),Priority!$B$85)</f>
+        <v>P3</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>28</v>
@@ -3359,7 +3376,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E20)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E20)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -3377,7 +3394,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E21)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E21)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -3394,9 +3411,9 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="str">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E22)&gt;0),Priority!$B$83)</f>
-        <v>P1</v>
+      <c r="B22" s="1" t="e">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E22)&gt;0),Priority!$B$85)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>79</v>
@@ -3413,7 +3430,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E23)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E23)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C23" s="12" t="s">
@@ -3431,7 +3448,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E24)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E24)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -3449,7 +3466,7 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E25)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E25)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -3467,7 +3484,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E26)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E26)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -3485,7 +3502,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E27)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E27)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -3503,7 +3520,7 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E28)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E28)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -3521,7 +3538,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E29)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E29)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C29" s="12" t="s">
@@ -3539,7 +3556,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E30)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E30)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -3557,7 +3574,7 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E31)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E31)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -3575,7 +3592,7 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E32)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E32)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -3593,7 +3610,7 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E33)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E33)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -3611,7 +3628,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E34)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E34)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C34" s="12" t="s">
@@ -3629,7 +3646,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E35)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E35)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -3647,7 +3664,7 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E36)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E36)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -3665,7 +3682,7 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E37)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E37)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C37" s="12" t="s">
@@ -3683,7 +3700,7 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E38)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E38)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C38" s="12" t="s">
@@ -3701,7 +3718,7 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E39)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E39)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C39" s="12" t="s">
@@ -3719,7 +3736,7 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E40)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E40)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C40" s="12" t="s">
@@ -3737,7 +3754,7 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E41)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E41)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -3755,7 +3772,7 @@
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E42)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E42)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C42" s="12" t="s">
@@ -3773,7 +3790,7 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E43)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E43)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -3791,7 +3808,7 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E44)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E44)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -3809,7 +3826,7 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E45)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E45)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -3827,7 +3844,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E46)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E46)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C46" s="12" t="s">
@@ -3845,7 +3862,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E47)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E47)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -3863,7 +3880,7 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E48)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E48)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C48" s="12" t="s">
@@ -3881,7 +3898,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E49)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E49)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -3903,7 +3920,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E50)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E50)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C50" s="12" t="s">
@@ -3921,7 +3938,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E51)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E51)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C51" s="12" t="s">
@@ -3939,7 +3956,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E52)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E52)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C52" s="12" t="s">
@@ -3957,7 +3974,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E53)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E53)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C53" s="12" t="s">
@@ -3975,7 +3992,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E54)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E54)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C54" s="12" t="s">
@@ -3993,7 +4010,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E55)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E55)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C55" s="12" t="s">
@@ -4011,7 +4028,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E56)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E56)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -4029,7 +4046,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E57)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E57)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C57" s="12" t="s">
@@ -4047,7 +4064,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E58)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E58)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -4065,7 +4082,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E59)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E59)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C59" s="12" t="s">
@@ -4083,7 +4100,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E60)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E60)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C60" s="12" t="s">
@@ -4101,7 +4118,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E61)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E61)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -4119,7 +4136,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E62)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E62)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C62" s="5" t="s">
@@ -4141,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E63)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E63)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C63" s="12" t="s">
@@ -4159,7 +4176,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E64)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E64)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C64" s="5" t="s">
@@ -4177,7 +4194,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E65)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E65)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -4195,7 +4212,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E66)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E66)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C66" s="12" t="s">
@@ -4213,7 +4230,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E67)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E67)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C67" s="12" t="s">
@@ -4231,7 +4248,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E68)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E68)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -4249,7 +4266,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E69)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E69)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -4269,7 +4286,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E70)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E70)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -4291,7 +4308,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E71)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E71)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -4313,7 +4330,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E72)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E72)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C72" s="5" t="s">
@@ -4335,7 +4352,7 @@
         <v>4</v>
       </c>
       <c r="B73" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E73)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E73)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C73" s="5" t="s">
@@ -4353,7 +4370,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E74)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E74)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C74" s="9" t="s">
@@ -4371,7 +4388,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E75)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E75)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C75" s="12" t="s">
@@ -4389,7 +4406,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E76)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E76)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C76" s="12" t="s">
@@ -4407,7 +4424,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E77)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E77)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C77" s="12" t="s">
@@ -4425,7 +4442,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E78)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E78)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C78" s="12" t="s">
@@ -4443,7 +4460,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E79)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E79)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -4461,7 +4478,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E80)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E80)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C80" s="12" t="s">
@@ -4479,7 +4496,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E81)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E81)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C81" s="15" t="s">
@@ -4497,7 +4514,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E82)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E82)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C82" s="12" t="s">
@@ -4515,7 +4532,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E83)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E83)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C83" s="5" t="s">
@@ -4533,7 +4550,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E84)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E84)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C84" s="12" t="s">
@@ -4551,7 +4568,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E85)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E85)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -4569,7 +4586,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E86)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E86)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C86" s="12" t="s">
@@ -4587,7 +4604,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E87)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E87)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C87" s="5" t="s">
@@ -4605,7 +4622,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E88)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E88)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C88" s="8" t="s">
@@ -4623,7 +4640,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E89)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E89)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C89" s="12" t="s">
@@ -4641,7 +4658,7 @@
     </row>
     <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E90)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E90)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C90" s="10" t="s">
@@ -4666,7 +4683,7 @@
         <v>1</v>
       </c>
       <c r="B91" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E91)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E91)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C91" s="12" t="s">
@@ -4684,7 +4701,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E92)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E92)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C92" s="5" t="s">
@@ -4701,9 +4718,9 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="str">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E93)&gt;0),Priority!$B$83)</f>
-        <v>P1</v>
+      <c r="B93" s="1" t="e">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E93)&gt;0),Priority!$B$85)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>142</v>
@@ -4719,9 +4736,9 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="1" t="str">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E94)&gt;0),Priority!$B$83)</f>
-        <v>P1</v>
+      <c r="B94" s="1" t="e">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E94)&gt;0),Priority!$B$85)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>61</v>
@@ -4738,7 +4755,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E95)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E95)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C95" s="12" t="s">
@@ -4756,7 +4773,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E96)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E96)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C96" s="12" t="s">
@@ -4774,7 +4791,7 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E97)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E97)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C97" s="12" t="s">
@@ -4792,7 +4809,7 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E98)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E98)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C98" s="12" t="s">
@@ -4810,7 +4827,7 @@
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E99)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E99)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -4828,7 +4845,7 @@
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E100)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E100)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C100" s="12" t="s">
@@ -4846,7 +4863,7 @@
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E101)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E101)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C101" s="12" t="s">
@@ -4864,7 +4881,7 @@
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E102)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E102)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C102" s="12" t="s">
@@ -4882,7 +4899,7 @@
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E103)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E103)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C103" s="12" t="s">
@@ -4900,7 +4917,7 @@
     </row>
     <row r="104" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E104)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E104)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C104" s="12"/>
@@ -4908,7 +4925,7 @@
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E105)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E105)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C105" s="13" t="s">
@@ -4926,7 +4943,7 @@
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E106)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E106)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C106" s="13" t="s">
@@ -4944,7 +4961,7 @@
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E107)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E107)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C107" s="13" t="s">
@@ -4962,7 +4979,7 @@
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E108)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E108)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C108" s="13" t="s">
@@ -4980,7 +4997,7 @@
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E109)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E109)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C109" s="13" t="s">
@@ -4997,9 +5014,9 @@
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E110)&gt;0),Priority!$B$83)</f>
-        <v>#VALUE!</v>
+      <c r="B110" s="1" t="str">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E110)&gt;0),Priority!$B$85)</f>
+        <v>P3</v>
       </c>
       <c r="C110" s="13" t="s">
         <v>282</v>
@@ -5016,7 +5033,7 @@
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E111)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E111)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C111" s="13" t="s">
@@ -5034,7 +5051,7 @@
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E112)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E112)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C112" s="13" t="s">
@@ -5051,9 +5068,9 @@
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E113)&gt;0),Priority!$B$83)</f>
-        <v>#VALUE!</v>
+      <c r="B113" s="1" t="str">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E113)&gt;0),Priority!$B$85)</f>
+        <v>P3</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>289</v>
@@ -5070,7 +5087,7 @@
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E114)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E114)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C114" s="13" t="s">
@@ -5088,7 +5105,7 @@
     </row>
     <row r="115" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E115)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E115)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C115" s="13"/>
@@ -5097,7 +5114,7 @@
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E116)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E116)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C116" s="13" t="s">
@@ -5114,9 +5131,9 @@
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B117" s="1" t="str">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E117)&gt;0),Priority!$B$83)</f>
-        <v>P1</v>
+      <c r="B117" s="1" t="e">
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E117)&gt;0),Priority!$B$85)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>304</v>
@@ -5133,7 +5150,7 @@
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E118)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E118)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C118" s="13" t="s">
@@ -5151,7 +5168,7 @@
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E119)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E119)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C119" s="13" t="s">
@@ -5169,7 +5186,7 @@
     </row>
     <row r="120" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E120)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E120)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C120" s="13" t="s">
@@ -5187,7 +5204,7 @@
     </row>
     <row r="121" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E121)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E121)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C121" s="13" t="s">
@@ -5205,7 +5222,7 @@
     </row>
     <row r="122" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E122)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E122)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C122" s="13" t="s">
@@ -5223,7 +5240,7 @@
     </row>
     <row r="123" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E123)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E123)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C123" s="13" t="s">
@@ -5241,7 +5258,7 @@
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E124)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E124)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C124" s="13" t="s">
@@ -5259,7 +5276,7 @@
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E125)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E125)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C125" s="13" t="s">
@@ -5277,7 +5294,7 @@
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E126)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E126)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C126" s="13" t="s">
@@ -5295,7 +5312,7 @@
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E127)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E127)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C127" s="13" t="s">
@@ -5313,7 +5330,7 @@
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E128)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E128)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C128" s="13" t="s">
@@ -5331,7 +5348,7 @@
     </row>
     <row r="129" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E129)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E129)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C129" s="13" t="s">
@@ -5349,7 +5366,7 @@
     </row>
     <row r="130" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E130)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E130)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C130" s="13" t="s">
@@ -5367,7 +5384,7 @@
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E131)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E131)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C131" s="13" t="s">
@@ -5385,7 +5402,7 @@
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E132)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E132)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C132" s="13" t="s">
@@ -5403,7 +5420,7 @@
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E133)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E133)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C133" s="13" t="s">
@@ -5421,7 +5438,7 @@
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E134)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E134)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C134" s="13" t="s">
@@ -5439,7 +5456,7 @@
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E135)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E135)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C135" s="13" t="s">
@@ -5457,7 +5474,7 @@
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E136)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E136)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C136" s="13" t="s">
@@ -5473,7 +5490,7 @@
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E137)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E137)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C137" s="13" t="s">
@@ -5491,7 +5508,7 @@
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E138)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E138)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C138" s="13" t="s">
@@ -5509,7 +5526,7 @@
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E139)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E139)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C139" s="13" t="s">
@@ -5527,7 +5544,7 @@
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E140)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E140)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C140" s="13" t="s">
@@ -5545,7 +5562,7 @@
     </row>
     <row r="141" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E141)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E141)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C141" s="13"/>
@@ -5554,14 +5571,14 @@
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E142)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E142)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C142" s="13"/>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E143)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E143)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C143" s="13" t="s">
@@ -5579,7 +5596,7 @@
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E144)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E144)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C144" s="13" t="s">
@@ -5597,7 +5614,7 @@
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E145)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E145)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C145" s="13" t="s">
@@ -5615,7 +5632,7 @@
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E146)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E146)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C146" s="13" t="s">
@@ -5633,7 +5650,7 @@
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E147)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E147)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C147" s="13" t="s">
@@ -5651,7 +5668,7 @@
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E148)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E148)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C148" s="13" t="s">
@@ -5669,7 +5686,7 @@
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E149)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E149)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C149" s="13" t="s">
@@ -5687,7 +5704,7 @@
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E150)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E150)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C150" s="13" t="s">
@@ -5705,7 +5722,7 @@
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E151)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E151)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C151" s="13" t="s">
@@ -5723,7 +5740,7 @@
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E152)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E152)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C152" s="13" t="s">
@@ -5741,7 +5758,7 @@
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E153)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E153)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C153" s="13" t="s">
@@ -5759,7 +5776,7 @@
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E154)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E154)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C154" s="13" t="s">
@@ -5777,7 +5794,7 @@
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E155)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E155)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C155" s="13" t="s">
@@ -5795,7 +5812,7 @@
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E156)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E156)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C156" s="13" t="s">
@@ -5813,7 +5830,7 @@
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E157)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E157)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C157" s="13" t="s">
@@ -5831,7 +5848,7 @@
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E158)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E158)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C158" s="13" t="s">
@@ -5849,7 +5866,7 @@
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="e">
-        <f>IF(OR(FIND(Priority!$B$34,Papers!E159)&gt;0),Priority!$B$83)</f>
+        <f>IF(OR(FIND(Priority!$B$79,Papers!E159)&gt;0),Priority!$B$85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C159" s="13" t="s">
@@ -5997,8 +6014,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A3:G86"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6046,7 +6063,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -6679,7 +6696,7 @@
     </row>
     <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>356</v>
@@ -6691,7 +6708,7 @@
     </row>
     <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>385</v>
@@ -6789,20 +6806,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="str">
         <f>IF(D69&gt;=5,$B$83,IF(D69=4,$B$84,$B$85))</f>
-        <v>P2</v>
+        <v>P3</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>344</v>
       </c>
       <c r="D69" s="1">
         <f>COUNTIF(Papers!E:E, "*"&amp;B69&amp;"*")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -6947,7 +6964,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>23</v>
@@ -6966,7 +6983,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -6974,7 +6991,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -6982,21 +6999,21 @@
         <v>4</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A9:D80">
     <filterColumn colId="3">
-      <colorFilter dxfId="1"/>
+      <colorFilter dxfId="2"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="A19:D79">
     <sortCondition descending="1" ref="D19:D79"/>
   </sortState>
   <conditionalFormatting sqref="D10:D80">
-    <cfRule type="top10" priority="1" rank="5"/>
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="top10" priority="2" rank="5"/>
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7008,10 +7025,11 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="top10" dxfId="0" priority="4" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="5" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="top10" priority="3" percent="1" rank="5"/>
+    <cfRule type="top10" dxfId="0" priority="1" rank="10"/>
+    <cfRule type="top10" priority="4" percent="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7039,23 +7057,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J57"/>
+  <dimension ref="A2:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="94.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
     <col min="4" max="4" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
@@ -7066,37 +7084,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -7113,88 +7112,95 @@
       <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>121</v>
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>122</v>
+        <v>224</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="7">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
+      <c r="A8" s="1">
+        <f>A7+1</f>
+        <v>2</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>214</v>
+        <v>151</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>145</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="7">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
+      <c r="A9" s="1">
+        <f t="shared" ref="A9:A47" si="0">A8+1</f>
+        <v>3</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>225</v>
+        <v>153</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>226</v>
+        <v>154</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="7">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>438</v>
+        <v>217</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="7">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>144</v>
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>123</v>
@@ -7205,71 +7211,75 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>67</v>
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>213</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>214</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="11">
-        <v>2007</v>
+      <c r="F12" s="7">
+        <v>2009</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="7">
-        <v>2007</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>118</v>
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>438</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="7">
-        <v>1999</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>340</v>
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>342</v>
+        <v>145</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="7">
@@ -7277,14 +7287,15 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>342</v>
@@ -7295,100 +7306,946 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="7">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="11">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="7">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="11">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="7">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="7">
+        <v>2008</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="7">
+        <v>2008</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="7">
+        <v>2008</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="11">
         <v>2007</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="7">
+        <v>2007</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="7">
+        <v>2007</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="7">
+        <v>2007</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="7">
+        <v>2006</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="7">
-        <v>2007</v>
+      <c r="B30" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="7">
+        <v>2006</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="7">
+        <v>2006</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="7">
+        <v>2006</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="7">
+        <v>2005</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="7">
+        <v>2004</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="11">
+        <v>2004</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="7">
+        <v>2003</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="7">
+        <v>2003</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="7">
+        <v>2002</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="7">
+        <v>2002</v>
+      </c>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="7">
+        <v>2002</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="11">
+        <v>2002</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="7">
+        <v>2001</v>
+      </c>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="11">
+        <v>2000</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="7">
+        <v>1999</v>
+      </c>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="7">
+        <v>1999</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A6:G6"/>
+  <sortState ref="A7:G47">
+    <sortCondition descending="1" ref="F6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>505</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="7">
+        <v>2003</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="7">
+        <v>2003</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="7">
+        <v>2002</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7">
+        <v>2006</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="7">
+        <v>2010</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="7">
+        <v>2010</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="7">
+        <v>2005</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="7">
+        <v>2009</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>307</v>
+        <v>499</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>309</v>
+        <v>169</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="7">
-        <v>2005</v>
-      </c>
+        <v>2008</v>
+      </c>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>499</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>346</v>
+        <v>301</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>348</v>
+        <v>302</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>347</v>
+        <v>303</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="7">
-        <v>2003</v>
-      </c>
+        <v>2010</v>
+      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>499</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>389</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>390</v>
+      </c>
       <c r="D21" s="14" t="s">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>426</v>
-      </c>
+        <v>1998</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="7">
+        <v>2002</v>
+      </c>
+      <c r="G22" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -7415,16 +8272,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>223</v>
+        <v>499</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>398</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>224</v>
+        <v>399</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>152</v>
+        <v>400</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="7">
@@ -7434,526 +8291,254 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>145</v>
+        <v>499</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>152</v>
+        <v>321</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="7">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>153</v>
+        <v>499</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>331</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>154</v>
+        <v>332</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>152</v>
+        <v>333</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="7">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>217</v>
+        <v>499</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>322</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>164</v>
+        <v>323</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>152</v>
+        <v>324</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="7">
-        <v>2010</v>
+        <v>2004</v>
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="7">
-        <v>2008</v>
-      </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="7">
-        <v>2008</v>
-      </c>
-      <c r="G30" s="1"/>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>505</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="14"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="7">
-        <v>2008</v>
-      </c>
+      <c r="F31" s="7"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="7">
-        <v>2006</v>
-      </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="7">
-        <v>2006</v>
-      </c>
-      <c r="G33" s="1"/>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>500</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="7">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>52</v>
+        <v>500</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>301</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>302</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>303</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="11">
-        <v>2004</v>
+      <c r="F35" s="7">
+        <v>2010</v>
       </c>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>500</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>387</v>
+        <v>389</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="7">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="11">
+        <v>2009</v>
+      </c>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="7">
+        <v>2005</v>
+      </c>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>70</v>
+        <v>500</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>289</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>71</v>
+        <v>291</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>290</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="11">
-        <v>2009</v>
+      <c r="F41" s="7">
+        <v>2003</v>
       </c>
       <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="7">
-        <v>2006</v>
-      </c>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="7">
-        <v>2006</v>
-      </c>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="7">
-        <v>2003</v>
-      </c>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="7">
-        <v>2002</v>
-      </c>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="7">
-        <v>2002</v>
-      </c>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="7">
-        <v>2002</v>
-      </c>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="11">
-        <v>2002</v>
-      </c>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="7">
-        <v>1999</v>
-      </c>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="7">
-        <v>2009</v>
-      </c>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="11">
-        <v>2009</v>
-      </c>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="7">
-        <v>2000</v>
-      </c>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E56" s="1"/>
-      <c r="F56" s="11">
-        <v>2000</v>
-      </c>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="E57" s="1"/>
-      <c r="F57" s="7">
-        <v>2009</v>
-      </c>
-      <c r="G57" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add abstract and summary to each paper (P1, P2, P3)
</commit_message>
<xml_diff>
--- a/State of Art_Text Detection & Recognition.xlsx
+++ b/State of Art_Text Detection & Recognition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="8475"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="8475" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Papers" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="596">
   <si>
     <t>Title</t>
   </si>
@@ -2827,6 +2827,80 @@
   </si>
   <si>
     <t>Most researchers have used edge, intensity, corner, and texture features for text localization in video images. However, these features do not fully coincide with the features of the text, and can not fulfill all the necessary conditions of the text. Therefore, it is very difficult to localize text robustly in video images which have complex backgrounds with strong edge or texture clutter using these features. In this paper, we propose a stroke filter which can detect strokes of texts for robust text localization. By using this stroke filter, we can remove text candidates which have strong edges but are not text. Furthermore, we apply the stroke filter to our text localization system and localize text more robustly in the video images. The effectiveness and efficiency of the proposed method is verified by extensive experiments on a challenging database containing 480 video images.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Mong muốn: rút trích những ký tự từ văn bản trong video, và sử dụng OCR để "đọc-nhận dạng" chúng; 2. Hiện thực: Khác với kỹ thuật truyền thống, tác giả chỉ rút trích những vùng văn băn đáng tin cậy dựa trên high-intensity, sau đó lấy ngưỡng trên những vùng này, và mở rộng thao tác trên toàn bộ những vùng văn bản trong video; 3. Tác giả claim: nó thì </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">tốt hơn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kỹ thuật truyền thống. 4. Dùng: màu sắc, và ngưỡng.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. xác định những đoạn line text tiềm năng từ dòng quét nằm ngang; kết hợp nó với những dòng quét lần cận để hình thành những block text lớn hơn; 2. Sau đó, nhị phân hóa mỗi vùng; 3. Sử dụng thuật toán làm nhịn đường viền, và nâng cao độ phân giải cải thiện chất lượng hình ảnh text; 4. Tác giả claim: thời gian thực thi nhân và hiệu quả trong những trường hợp phức tạp. 5. Thao tác xác định: đoạn line text tiềm năng ra sao?</t>
+  </si>
+  <si>
+    <t>1. Hướng tiếp cận đa phân giải trong việc định vị và phân đoạn text trong video. Không biết kỹ thuật thế nào?; 2. Claim: định vị chính xác 95% đoạn văn bản trong video, phân đoạn chính xác 80% các ký tự trong các đoạn văn, 7.8% các ký tự không phân đoạn được, 90% các ký tự sau khi phân đươc nhận dạng chĩnh xác bởi OCR chuẩn</t>
+  </si>
+  <si>
+    <t>potential</t>
+  </si>
+  <si>
+    <t>1. xác định vùng văn bản bằng việc dùng wavlet decomposition and di chuyển giả của các ảnh. 2. Ý tượng: khi ảnh tĩnh dịch chuyển, các hệ số wavelet của nó sẽ dao dộng. Tác giả dụng đặc tính này để định vị văn bản trong ảnh</t>
+  </si>
+  <si>
+    <t>1. Dùng đặc trưng texture cho việc phân đoạn những vùng văn bản khỏi background trên miền nén DCT; 2. Tinh chỉnh thêm chúng trên miền không gian; Kết quả: tỉ lệ reject sai 4% nhỏ hơn tỉ lệ chấp nhận sai  5.7%</t>
+  </si>
+  <si>
+    <t>Vân</t>
+  </si>
+  <si>
+    <t>cạnh, nhị phân hóa,  làm mịn đường viền và nâng cao chất lượng văn bản với morphology</t>
+  </si>
+  <si>
+    <t>đa phân giải ra sao? Mà claim ghê quá</t>
+  </si>
+  <si>
+    <t>kỹ thuật tương tối phức tạp, chúng liên quan tới xác suất</t>
+  </si>
+  <si>
+    <t>chuyển động giả, wavelet decomposition, hệ số wavelet</t>
+  </si>
+  <si>
+    <t>1. Mục đích: Phát hiện văn bản để phục vụ cho việc chỉ mục và truy vấn thông tin video; 2. Hiện thực: dùng các đặc trưng bất biến như: độ đậm của cạnh, mật độ cạnh và phân phối chiều ngang; 3. Các bước: a)dò tìm những cạnh đậm nét; b)nhị phân hóa ảnh với ngưỡng cục bộ; c) nâng cao chất lượng văn bản với hai thao tác làm nổi bật đường nét cạnh và mật độ cạnh; d) cuối cùng, định vị văn bản theo cách dò từ thô tới mịn</t>
+  </si>
+  <si>
+    <t>cạnh: đường nét, mật độ, và phân bố theo chiều ngang của nó</t>
+  </si>
+  <si>
+    <t>cách làm tương đối rõ</t>
+  </si>
+  <si>
+    <t>Màu sắc, ngưỡng, làm thế nào biết vùng văn bản có cường độ cao</t>
+  </si>
+  <si>
+    <t>Cùng mục đích như paper 35. 1)Hai thách thức của VCR: độ phân giải thấp, và background phức tạp. 2) Ý tượng: dùng nhiều frame trong video mà chứa cùng văn bản để làm rõ mỗi từ. 3)Các bước: xác định và chọn ra những frame chứa văn băn gần giống nhau; b) dò tìm và hợp những khối text từ những frame này và hình thành một frame "man-made" rõ hơn; c) lấy ngưỡng, nhị phân hóa frame và đưa vào OCR để nhận dạng</t>
+  </si>
+  <si>
+    <t>kỹ thuật dò tìm những block text trong đây như thế nào?  Cụ thể hơn, không rõ đặc trưng được dùng để detect text block</t>
   </si>
 </sst>
 </file>
@@ -2902,7 +2976,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2912,6 +2986,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2929,7 +3009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2999,6 +3079,19 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3332,8 +3425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B73" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6740,18 +6833,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="5" max="5" width="2.42578125" customWidth="1"/>
     <col min="7" max="7" width="46.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7400,7 +7495,7 @@
       </c>
       <c r="H32" s="17"/>
     </row>
-    <row r="33" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -7423,7 +7518,7 @@
       </c>
       <c r="H33" s="17"/>
     </row>
-    <row r="34" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7446,7 +7541,7 @@
       </c>
       <c r="H34" s="17"/>
     </row>
-    <row r="35" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7469,7 +7564,7 @@
       </c>
       <c r="H35" s="17"/>
     </row>
-    <row r="36" spans="1:8" ht="345" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7492,7 +7587,7 @@
       </c>
       <c r="H36" s="17"/>
     </row>
-    <row r="37" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7515,7 +7610,7 @@
       </c>
       <c r="H37" s="17"/>
     </row>
-    <row r="38" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7538,7 +7633,7 @@
       </c>
       <c r="H38" s="17"/>
     </row>
-    <row r="39" spans="1:8" ht="375" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="375" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7561,7 +7656,7 @@
       </c>
       <c r="H39" s="17"/>
     </row>
-    <row r="40" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7582,9 +7677,17 @@
       <c r="G40" s="17" t="s">
         <v>526</v>
       </c>
-      <c r="H40" s="17"/>
-    </row>
-    <row r="41" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+      <c r="H40" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="J40" s="17" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7605,9 +7708,17 @@
       <c r="G41" s="17" t="s">
         <v>525</v>
       </c>
-      <c r="H41" s="17"/>
-    </row>
-    <row r="42" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+      <c r="H41" s="17" t="s">
+        <v>590</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="J41" s="17" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7626,32 +7737,42 @@
       <c r="G42" s="17" t="s">
         <v>524</v>
       </c>
-      <c r="H42" s="17"/>
-    </row>
-    <row r="43" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+      <c r="H42" s="17" t="s">
+        <v>583</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="35" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="32" t="s">
         <v>386</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="32" t="s">
         <v>387</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="33" t="s">
         <v>388</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="21">
+      <c r="E43" s="31"/>
+      <c r="F43" s="34">
         <v>2000</v>
       </c>
-      <c r="G43" s="17" t="s">
+      <c r="G43" s="31" t="s">
         <v>523</v>
       </c>
-      <c r="H43" s="17"/>
-    </row>
-    <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="I43" s="31" t="s">
+        <v>588</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7672,9 +7793,17 @@
       <c r="G44" s="17" t="s">
         <v>522</v>
       </c>
-      <c r="H44" s="17"/>
-    </row>
-    <row r="45" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+      <c r="H44" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>587</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="315" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7695,9 +7824,14 @@
       <c r="G45" s="17" t="s">
         <v>521</v>
       </c>
-      <c r="H45" s="17"/>
-    </row>
-    <row r="46" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="H45" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="315" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -7718,9 +7852,14 @@
       <c r="G46" s="17" t="s">
         <v>519</v>
       </c>
-      <c r="H46" s="17"/>
-    </row>
-    <row r="47" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="H46" s="17" t="s">
+        <v>579</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -7741,7 +7880,12 @@
       <c r="G47" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="H47" s="17"/>
+      <c r="H47" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>585</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A6:H6"/>
@@ -7770,8 +7914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>